<commit_message>
Final (?) Risk Profiler
</commit_message>
<xml_diff>
--- a/resources/risk_profiler.xlsx
+++ b/resources/risk_profiler.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="9">
   <si>
     <t>TOTAL</t>
   </si>
@@ -165,14 +165,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
@@ -491,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,216 +510,281 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2">
+        <v>2</v>
+      </c>
+      <c r="N3" s="2">
+        <v>3</v>
+      </c>
+      <c r="O3" s="2">
+        <v>4</v>
+      </c>
+      <c r="P3" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="C4" s="2">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3">
+      <c r="K4" s="2">
+        <v>5</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
+        <v>0</v>
+      </c>
+      <c r="O4" s="7">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="3">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2">
+        <v>4</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="N5" s="7">
+        <v>0</v>
+      </c>
+      <c r="O5" s="7">
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
+      <c r="K6" s="2">
+        <v>3</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
+        <v>0</v>
+      </c>
+      <c r="O6" s="7">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C7" s="2"/>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="3">
-        <v>0</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0</v>
-      </c>
-      <c r="N7" s="3">
-        <v>0</v>
-      </c>
-      <c r="O7" s="3">
-        <v>0</v>
-      </c>
-      <c r="P7" s="3">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2">
+        <v>2</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="7">
+        <v>0</v>
+      </c>
+      <c r="P7" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="3">
-        <v>0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>0</v>
-      </c>
-      <c r="N8" s="3">
-        <v>0</v>
-      </c>
-      <c r="O8" s="3">
-        <v>0</v>
-      </c>
-      <c r="P8" s="3">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
+        <v>0</v>
+      </c>
+      <c r="N8" s="7">
+        <v>0</v>
+      </c>
+      <c r="O8" s="7">
+        <v>0</v>
+      </c>
+      <c r="P8" s="7">
         <v>0</v>
       </c>
     </row>
@@ -728,10 +800,6 @@
       <c r="H9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I9">
-        <f>SUM(D4:H8)</f>
-        <v>0</v>
-      </c>
       <c r="L9" s="2" t="s">
         <v>4</v>
       </c>
@@ -742,143 +810,158 @@
       <c r="P9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q9">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <f>SUM(D4:H8)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
         <f>SUM(L4:P8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D12">
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>4</v>
+      </c>
+      <c r="H12" s="2">
         <v>5</v>
       </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>2</v>
+      </c>
+      <c r="N12" s="2">
         <v>3</v>
       </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="L12">
+      <c r="O12" s="2">
+        <v>4</v>
+      </c>
+      <c r="P12" s="2">
         <v>5</v>
-      </c>
-      <c r="M12">
-        <v>4</v>
-      </c>
-      <c r="N12">
-        <v>3</v>
-      </c>
-      <c r="O12">
-        <v>2</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>5</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="8">
         <f t="shared" ref="D13:H17" si="0">$C13*D$12*D4</f>
         <v>0</v>
       </c>
-      <c r="E13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="2">
         <v>5</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="8">
         <f t="shared" ref="L13:P17" si="1">$C13*L$12*L4</f>
         <v>0</v>
       </c>
-      <c r="M13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="4">
+      <c r="M13" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
+      <c r="C14" s="2">
+        <v>4</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J14" s="2"/>
-      <c r="K14">
-        <v>4</v>
-      </c>
-      <c r="L14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="4">
+      <c r="K14" s="2">
+        <v>4</v>
+      </c>
+      <c r="L14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -887,102 +970,102 @@
       <c r="B15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>3</v>
       </c>
-      <c r="D15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
+      <c r="D15" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="2">
         <v>3</v>
       </c>
-      <c r="L15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="4">
+      <c r="L15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>2</v>
       </c>
-      <c r="D16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
+      <c r="D16" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J16" s="2"/>
-      <c r="K16">
+      <c r="K16" s="2">
         <v>2</v>
       </c>
-      <c r="L16" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="4">
+      <c r="L16" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -991,52 +1074,52 @@
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>1</v>
       </c>
-      <c r="D17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
+      <c r="D17" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="2">
         <v>1</v>
       </c>
-      <c r="L17" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="4">
+      <c r="L17" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1064,39 +1147,52 @@
         <v>5</v>
       </c>
     </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <f>SUM(D13:H17)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5">
+        <f>SUM(L13:P17)</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I20" s="7">
-        <f>SUM(D13:H17)</f>
-        <v>0</v>
-      </c>
-      <c r="P20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="7">
-        <f>SUM(L13:P17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H21" s="5" t="s">
+      <c r="H20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I21" s="6" t="str">
-        <f>IF(I20&lt;&gt;0,I20/I9,"0")</f>
-        <v>0</v>
-      </c>
-      <c r="P21" s="5" t="s">
+      <c r="I20" s="6" t="str">
+        <f>IF(I19&lt;&gt;0,I19/I10,"0")</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="Q21" s="6" t="str">
-        <f>IF(Q20&lt;&gt;0,Q20/Q9,"0")</f>
+      <c r="Q20" s="6" t="str">
+        <f>IF(Q19&lt;&gt;0,Q19/Q10,"0")</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="xpO8rOEmrdeU04Lxj4iCbhpmS5639VKdkeL1ZYJBJWxPV3y0WxeRxeYZJubYttAS5hZmMhyL3BCKKZhySkJUnA==" saltValue="76Xg10+37oplj/p7feGBGg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="D13:H17">
     <cfRule type="colorScale" priority="2">
       <colorScale>

</xml_diff>